<commit_message>
updated true value calculations
</commit_message>
<xml_diff>
--- a/Results/Sim_results/JM_ests_by_scenario.xlsx
+++ b/Results/Sim_results/JM_ests_by_scenario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Scenario</t>
   </si>
@@ -88,18 +88,6 @@
   </si>
   <si>
     <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adj_time^2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time^2</t>
   </si>
 </sst>
 </file>
@@ -790,19 +778,19 @@
         <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>51.9723424612926</v>
+        <v>47.6427512472055</v>
       </c>
       <c r="E13" t="n">
         <v>50.0132664025535</v>
       </c>
       <c r="F13" t="n">
-        <v>3.95685120930715</v>
+        <v>5.73821430711651</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.95907605873912</v>
+        <v>2.37051515534792</v>
       </c>
       <c r="H13" t="n">
-        <v>-3.76945884284162</v>
+        <v>4.9756050884802</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -819,19 +807,19 @@
         <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>51.9723424612926</v>
+        <v>47.6427512472055</v>
       </c>
       <c r="E14" t="n">
         <v>50.0113015018857</v>
       </c>
       <c r="F14" t="n">
-        <v>3.96501552992363</v>
+        <v>5.72936419439771</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.96104095940687</v>
+        <v>2.36855025468017</v>
       </c>
       <c r="H14" t="n">
-        <v>-3.77323950881644</v>
+        <v>4.97148085002564</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1384,22 +1372,22 @@
         <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>49.9464303063664</v>
+        <v>45.6385571388249</v>
       </c>
       <c r="E13" t="n">
         <v>47.6149991709379</v>
       </c>
       <c r="F13" t="n">
-        <v>5.66422514455855</v>
+        <v>4.13497711161598</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.33143113542849</v>
+        <v>1.97644203211296</v>
       </c>
       <c r="H13" t="n">
-        <v>-4.66786339109267</v>
+        <v>4.33064092298306</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="14">
@@ -1413,22 +1401,22 @@
         <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>49.9464303063664</v>
+        <v>45.6385571388249</v>
       </c>
       <c r="E14" t="n">
         <v>47.6239910640183</v>
       </c>
       <c r="F14" t="n">
-        <v>5.62231434908653</v>
+        <v>4.17053818599683</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.3224392423481</v>
+        <v>1.98543392519335</v>
       </c>
       <c r="H14" t="n">
-        <v>-4.64986031654813</v>
+        <v>4.35034332736241</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="15">
@@ -1659,22 +1647,22 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.14858749195492</v>
+        <v>-1.17816064114501</v>
       </c>
       <c r="E2" t="n">
         <v>-1.13757402422165</v>
       </c>
       <c r="F2" t="n">
-        <v>0.000560254185514937</v>
+        <v>0.00208623118728726</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0110134677332696</v>
+        <v>0.0405866169233664</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.958870596311692</v>
+        <v>-3.44491366507726</v>
       </c>
       <c r="I2" t="n">
-        <v>0.942</v>
+        <v>0.582</v>
       </c>
     </row>
     <row r="3">
@@ -1688,22 +1676,22 @@
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.14858749195492</v>
+        <v>-1.17816064114501</v>
       </c>
       <c r="E3" t="n">
         <v>-1.1409788346877</v>
       </c>
       <c r="F3" t="n">
-        <v>0.000502558940555886</v>
+        <v>0.00182715400657475</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00760865726721183</v>
+        <v>0.0371818064573086</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.662436019937998</v>
+        <v>-3.1559199279627</v>
       </c>
       <c r="I3" t="n">
-        <v>0.956</v>
+        <v>0.638</v>
       </c>
     </row>
     <row r="4">
@@ -1978,19 +1966,19 @@
         <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>48.6008464519665</v>
+        <v>43.2641357790691</v>
       </c>
       <c r="E13" t="n">
         <v>45.8502509724383</v>
       </c>
       <c r="F13" t="n">
-        <v>7.81130221669589</v>
+        <v>6.93351851807055</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.75059547952812</v>
+        <v>2.58611519336923</v>
       </c>
       <c r="H13" t="n">
-        <v>-5.65956290956085</v>
+        <v>5.97750341431846</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -2007,19 +1995,19 @@
         <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>48.6008464519665</v>
+        <v>43.2641357790691</v>
       </c>
       <c r="E14" t="n">
         <v>45.861553523349</v>
       </c>
       <c r="F14" t="n">
-        <v>7.74819178803776</v>
+        <v>6.99104497756438</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.73929292861744</v>
+        <v>2.59741774427991</v>
       </c>
       <c r="H14" t="n">
-        <v>-5.63630703700759</v>
+        <v>6.00362794149819</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -2152,22 +2140,22 @@
         <v>14</v>
       </c>
       <c r="D19" t="n">
-        <v>-1.14858749195492</v>
+        <v>-1.17816064114501</v>
       </c>
       <c r="E19" t="n">
         <v>-1.13816262011739</v>
       </c>
       <c r="F19" t="n">
-        <v>0.000504086440137612</v>
+        <v>0.00199525017343497</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0104248718375268</v>
+        <v>0.0399980210276236</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.907625401682157</v>
+        <v>-3.3949547821213</v>
       </c>
       <c r="I19" t="n">
-        <v>0.936</v>
+        <v>0.532</v>
       </c>
     </row>
     <row r="20">
@@ -2181,22 +2169,22 @@
         <v>15</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.14858749195492</v>
+        <v>-1.17816064114501</v>
       </c>
       <c r="E20" t="n">
         <v>-1.13730463881024</v>
       </c>
       <c r="F20" t="n">
-        <v>0.000521658904245191</v>
+        <v>0.00206356905593969</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0112828531446738</v>
+        <v>0.0408560023347706</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.982324222029459</v>
+        <v>-3.46777857857007</v>
       </c>
       <c r="I20" t="n">
-        <v>0.929</v>
+        <v>0.508</v>
       </c>
     </row>
   </sheetData>
@@ -2572,22 +2560,22 @@
         <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>50.9654237458654</v>
+        <v>47.0947655936096</v>
       </c>
       <c r="E13" t="n">
         <v>48.7672088641827</v>
       </c>
       <c r="F13" t="n">
-        <v>5.03416014006206</v>
+        <v>2.99907796729558</v>
       </c>
       <c r="G13" t="n">
-        <v>-2.19821488168277</v>
+        <v>1.67244327057306</v>
       </c>
       <c r="H13" t="n">
-        <v>-4.31314942586169</v>
+        <v>3.5512296313457</v>
       </c>
       <c r="I13" t="n">
-        <v>0.001</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="14">
@@ -2601,22 +2589,22 @@
         <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>50.9654237458654</v>
+        <v>47.0947655936096</v>
       </c>
       <c r="E14" t="n">
         <v>48.7773531186157</v>
       </c>
       <c r="F14" t="n">
-        <v>4.9899607932187</v>
+        <v>3.03340850269197</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.18807062724972</v>
+        <v>1.68258752500612</v>
       </c>
       <c r="H14" t="n">
-        <v>-4.29324523653592</v>
+        <v>3.57276972036662</v>
       </c>
       <c r="I14" t="n">
-        <v>0.001</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="15">
@@ -2879,38 +2867,58 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4"/>
+        <v>14</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.05</v>
+      </c>
       <c r="E4" t="n">
-        <v>-118.485526511134</v>
-      </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
+        <v>-0.0639900501037536</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.00024366913351453</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.0139900501037536</v>
+      </c>
+      <c r="H4" t="n">
+        <v>27.9801002075072</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.384</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5"/>
+        <v>15</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.05</v>
+      </c>
       <c r="E5" t="n">
-        <v>96.4361829930472</v>
-      </c>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
+        <v>-0.0678232339187681</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.000357275084565115</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-0.0178232339187681</v>
+      </c>
+      <c r="H5" t="n">
+        <v>35.6464678375363</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -2920,25 +2928,25 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
         <v>-0.05</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.0639900501037536</v>
+        <v>-0.0251897054763717</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00024366913351453</v>
+        <v>0.000637390711045616</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0139900501037536</v>
+        <v>0.0248102945236283</v>
       </c>
       <c r="H6" t="n">
-        <v>27.9801002075072</v>
+        <v>-49.6205890472566</v>
       </c>
       <c r="I6" t="n">
-        <v>0.384</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="7">
@@ -2949,25 +2957,25 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" t="n">
         <v>-0.05</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0678232339187681</v>
+        <v>-0.0643143100739772</v>
       </c>
       <c r="F7" t="n">
-        <v>0.000357275084565115</v>
+        <v>0.000246582516983309</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0178232339187681</v>
+        <v>-0.0143143100739772</v>
       </c>
       <c r="H7" t="n">
-        <v>35.6464678375363</v>
+        <v>28.6286201479544</v>
       </c>
       <c r="I7" t="n">
-        <v>0.17</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="8">
@@ -2975,28 +2983,28 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
         <v>-0.05</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0251897054763717</v>
+        <v>-0.0742941028317831</v>
       </c>
       <c r="F8" t="n">
-        <v>0.000637390711045616</v>
+        <v>0.000620266190438527</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0248102945236283</v>
+        <v>-0.0242941028317831</v>
       </c>
       <c r="H8" t="n">
-        <v>-49.6205890472566</v>
+        <v>48.5882056635662</v>
       </c>
       <c r="I8" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="9">
@@ -3004,28 +3012,28 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D9" t="n">
         <v>-0.05</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0643143100739772</v>
+        <v>-0.0493802802626681</v>
       </c>
       <c r="F9" t="n">
-        <v>0.000246582516983309</v>
+        <v>0.0000379159968074252</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0143143100739772</v>
+        <v>0.000619719737331874</v>
       </c>
       <c r="H9" t="n">
-        <v>28.6286201479544</v>
+        <v>-1.23943947466375</v>
       </c>
       <c r="I9" t="n">
-        <v>0.34</v>
+        <v>0.929</v>
       </c>
     </row>
     <row r="10">
@@ -3033,28 +3041,28 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D10" t="n">
         <v>-0.05</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0493545712454893</v>
+        <v>-0.0599400941925494</v>
       </c>
       <c r="F10" t="n">
-        <v>0.000054616325885854</v>
+        <v>0.000140613920358508</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00064542875451068</v>
+        <v>-0.00994009419254935</v>
       </c>
       <c r="H10" t="n">
-        <v>-1.29085750902136</v>
+        <v>19.8801883850987</v>
       </c>
       <c r="I10" t="n">
-        <v>0.907</v>
+        <v>0.619</v>
       </c>
     </row>
     <row r="11">
@@ -3062,28 +3070,28 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.05</v>
+        <v>60</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0417740570332573</v>
+        <v>45.1316671554835</v>
       </c>
       <c r="F11" t="n">
-        <v>0.000110408994073717</v>
+        <v>221.246412095971</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00822594296674273</v>
+        <v>-14.8683328445165</v>
       </c>
       <c r="H11" t="n">
-        <v>-16.4518859334855</v>
+        <v>-24.7805547408608</v>
       </c>
       <c r="I11" t="n">
-        <v>0.669</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -3091,28 +3099,28 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.05</v>
+        <v>60</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.0742941028317831</v>
+        <v>45.0888707533345</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000620266190438527</v>
+        <v>222.521494189103</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.0242941028317831</v>
+        <v>-14.9111292466655</v>
       </c>
       <c r="H12" t="n">
-        <v>48.5882056635662</v>
+        <v>-24.8518820777758</v>
       </c>
       <c r="I12" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -3120,28 +3128,28 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.05</v>
+        <v>60.9486402820125</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.0493802802626681</v>
+        <v>33.692802534035</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0000379159968074252</v>
+        <v>743.098405938023</v>
       </c>
       <c r="G13" t="n">
-        <v>0.000619719737331874</v>
+        <v>-27.2558377479775</v>
       </c>
       <c r="H13" t="n">
-        <v>-1.23943947466375</v>
+        <v>-44.7193532486751</v>
       </c>
       <c r="I13" t="n">
-        <v>0.929</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -3149,28 +3157,28 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.05</v>
+        <v>60.9486402820125</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0599400941925494</v>
+        <v>33.7435332854168</v>
       </c>
       <c r="F14" t="n">
-        <v>0.000140613920358508</v>
+        <v>740.335530562616</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.00994009419254935</v>
+        <v>-27.2051069965957</v>
       </c>
       <c r="H14" t="n">
-        <v>19.8801883850987</v>
+        <v>-44.6361180015112</v>
       </c>
       <c r="I14" t="n">
-        <v>0.619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -3178,28 +3186,28 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.05</v>
+        <v>0.405465108108164</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.0519681671667667</v>
+        <v>0.440043946226306</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0000387001773646441</v>
+        <v>0.00957081063519616</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.00196816716676673</v>
+        <v>0.0345788381181418</v>
       </c>
       <c r="H15" t="n">
-        <v>3.93633433353345</v>
+        <v>8.52819081757272</v>
       </c>
       <c r="I15" t="n">
-        <v>0.925</v>
+        <v>0.904</v>
       </c>
     </row>
     <row r="16">
@@ -3207,28 +3215,28 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.05</v>
+        <v>0.405465108108164</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.0431620092317713</v>
+        <v>0.415411524321704</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0000858146558034104</v>
+        <v>0.00764765594420519</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0068379907682287</v>
+        <v>0.00994641621353914</v>
       </c>
       <c r="H16" t="n">
-        <v>-13.6759815364574</v>
+        <v>2.45308807456887</v>
       </c>
       <c r="I16" t="n">
-        <v>0.774</v>
+        <v>0.935</v>
       </c>
     </row>
     <row r="17">
@@ -3236,28 +3244,28 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>60</v>
+        <v>0.405465108108164</v>
       </c>
       <c r="E17" t="n">
-        <v>45.1316671554835</v>
+        <v>0.393092431613081</v>
       </c>
       <c r="F17" t="n">
-        <v>221.246412095971</v>
+        <v>0.00767518190681472</v>
       </c>
       <c r="G17" t="n">
-        <v>-14.8683328445165</v>
+        <v>-0.0123726764950832</v>
       </c>
       <c r="H17" t="n">
-        <v>-24.7805547408608</v>
+        <v>-3.05147748786872</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>0.945</v>
       </c>
     </row>
     <row r="18">
@@ -3265,28 +3273,28 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>60</v>
+        <v>0.405465108108164</v>
       </c>
       <c r="E18" t="n">
-        <v>45.0888707533345</v>
+        <v>0.416223591102119</v>
       </c>
       <c r="F18" t="n">
-        <v>222.521494189103</v>
+        <v>0.00760595435892283</v>
       </c>
       <c r="G18" t="n">
-        <v>-14.9111292466655</v>
+        <v>0.0107584829939544</v>
       </c>
       <c r="H18" t="n">
-        <v>-24.8518820777758</v>
+        <v>2.65336838579076</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>0.935</v>
       </c>
     </row>
     <row r="19">
@@ -3294,366 +3302,38 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="n">
-        <v>37.6013011890765</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D19"/>
       <c r="E19" t="n">
-        <v>33.692802534035</v>
-      </c>
-      <c r="F19" t="n">
-        <v>15.4940763304107</v>
-      </c>
-      <c r="G19" t="n">
-        <v>-3.90849865504143</v>
-      </c>
-      <c r="H19" t="n">
-        <v>-10.394583515575</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
+        <v>-1.03764050970361</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="n">
-        <v>37.6013011890765</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D20"/>
       <c r="E20" t="n">
-        <v>33.7435332854168</v>
-      </c>
-      <c r="F20" t="n">
-        <v>15.1000570649034</v>
-      </c>
-      <c r="G20" t="n">
-        <v>-3.85776790365965</v>
-      </c>
-      <c r="H20" t="n">
-        <v>-10.2596659734221</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" t="n">
-        <v>60</v>
-      </c>
-      <c r="E21" t="n">
-        <v>36.535230220027</v>
-      </c>
-      <c r="F21" t="n">
-        <v>551.47539082805</v>
-      </c>
-      <c r="G21" t="n">
-        <v>-23.464769779973</v>
-      </c>
-      <c r="H21" t="n">
-        <v>-39.1079496332884</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" t="n">
-        <v>37.6013011890765</v>
-      </c>
-      <c r="E22" t="n">
-        <v>25.3587930017327</v>
-      </c>
-      <c r="F22" t="n">
-        <v>150.472359989378</v>
-      </c>
-      <c r="G22" t="n">
-        <v>-12.2425081873437</v>
-      </c>
-      <c r="H22" t="n">
-        <v>-32.5587354697722</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.405465108108164</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.440043946226306</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.00957081063519616</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.0345788381181418</v>
-      </c>
-      <c r="H23" t="n">
-        <v>8.52819081757272</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0.904</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.405465108108164</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.415411524321704</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.00764765594420519</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.00994641621353914</v>
-      </c>
-      <c r="H24" t="n">
-        <v>2.45308807456887</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0.935</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.405465108108164</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.393092431613081</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.00767518190681472</v>
-      </c>
-      <c r="G25" t="n">
-        <v>-0.0123726764950832</v>
-      </c>
-      <c r="H25" t="n">
-        <v>-3.05147748786872</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0.945</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.405465108108164</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.416223591102119</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.00760595435892283</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.0107584829939544</v>
-      </c>
-      <c r="H26" t="n">
-        <v>2.65336838579076</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.935</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0.405465108108164</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.411268142323335</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.00729470207004713</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.00580303421517037</v>
-      </c>
-      <c r="H27" t="n">
-        <v>1.43120433771636</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0.944</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.405465108108164</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.40571005831823</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0.00706436208155754</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.000244950210065209</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0.0604121551193659</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0.948</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29"/>
-      <c r="E29" t="n">
-        <v>-1.03764050970361</v>
-      </c>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30"/>
-      <c r="E30" t="n">
         <v>-1.03690428834515</v>
       </c>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31"/>
-      <c r="E31" t="n">
-        <v>-91.2696769629217</v>
-      </c>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32"/>
-      <c r="E32" t="n">
-        <v>136.400533966067</v>
-      </c>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>